<commit_message>
adicionando filtro pelo log
</commit_message>
<xml_diff>
--- a/database/question.xlsx
+++ b/database/question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B45A7D-92A3-4F59-B962-157A4C8709C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AB1F77-C7D0-40C8-A16D-572ED10B89ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3EFBC443-D211-4DB2-832F-973E0CDB4A3C}"/>
   </bookViews>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4B775F-9670-46A2-A8C1-55D3CF8BF806}">
   <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adicionando perguntas filtro, faltando apenas ler a resposta da pergunta
</commit_message>
<xml_diff>
--- a/database/question.xlsx
+++ b/database/question.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herik\OneDrive\Área de Trabalho\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC08EC1D-5F1B-4EEA-8B25-B6E403011FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D2B08A-BFD9-4CD9-BDEC-C3A20C52E981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3EFBC443-D211-4DB2-832F-973E0CDB4A3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3EFBC443-D211-4DB2-832F-973E0CDB4A3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>não tenho certeza se entendi corretamente. Você poderia confirmar se o problema que você está enfrentando é sobre: _?</t>
-  </si>
-  <si>
     <t>question_doubt</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>question_options</t>
+  </si>
+  <si>
+    <t>não tenho certeza se entendi corretamente. Você poderia confirmar se o problema que você está enfrentando é sobre _?</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,24 +472,24 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>